<commit_message>
demostracion de evidencia final
</commit_message>
<xml_diff>
--- a/test_docs/QA_Proyecto_LoginRegistro_TestCases_Bugs.xlsx
+++ b/test_docs/QA_Proyecto_LoginRegistro_TestCases_Bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\qa_test_project\test_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E143E748-25FF-43CC-8AAF-91F74D70C270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6DA367-B995-47F9-A090-B31372C097BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E66617BC-C8B3-4F4A-AF59-3723FF5A4E16}"/>
   </bookViews>
@@ -177,13 +177,6 @@
     <t>Validar que el sistema muestre mensaje adecuado cuando la contraseña sea incorrecta.</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1. Abrir http://localhost/qa_test_project/login.php
-2. Ingresar:
- - Email: juan@test.com
- - Contraseña: 891011
-3. Pulsar “Ingresar”.</t>
-  </si>
-  <si>
     <t>Email: ulisesn@test.com
 Contraseña: 891011</t>
   </si>
@@ -288,6 +281,13 @@
   <si>
     <t>Mostrar mensaje “El email ya está registrado”.
 No insertar nuevo registro en la base de datos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Abrir http://localhost/qa_test_project/login.php
+2. Ingresar:
+ - Email: ulisesn@test.com
+ - Contraseña: 891011
+3. Pulsar “Ingresar”.</t>
   </si>
 </sst>
 </file>
@@ -834,8 +834,8 @@
   </sheetPr>
   <dimension ref="A2:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +936,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>24</v>
@@ -994,54 +994,54 @@
         <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1057,7 +1057,7 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -1089,13 +1089,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>5</v>
@@ -1104,42 +1104,42 @@
         <v>6</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="I3" s="21" t="s">
         <v>64</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>65</v>
       </c>
       <c r="J3" s="20"/>
     </row>

</xml_diff>

<commit_message>
test docs qa correccion
</commit_message>
<xml_diff>
--- a/test_docs/QA_Proyecto_LoginRegistro_TestCases_Bugs.xlsx
+++ b/test_docs/QA_Proyecto_LoginRegistro_TestCases_Bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\qa_test_project\test_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6DA367-B995-47F9-A090-B31372C097BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261ABF21-20D6-4FD9-B6A6-CB608B8CB5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E66617BC-C8B3-4F4A-AF59-3723FF5A4E16}"/>
   </bookViews>
@@ -835,7 +835,7 @@
   <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>